<commit_message>
maj nomenclature et  ajout des demandes de modif et etc.
</commit_message>
<xml_diff>
--- a/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
+++ b/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>ID du projet</t>
   </si>
@@ -67,6 +67,24 @@
   </si>
   <si>
     <t>Equipe 2</t>
+  </si>
+  <si>
+    <t>David Paquet</t>
+  </si>
+  <si>
+    <t>CodeSysExp de varchar(10) à varchar(20)</t>
+  </si>
+  <si>
+    <t>DA1</t>
+  </si>
+  <si>
+    <t>GA01</t>
+  </si>
+  <si>
+    <t>Gabriel Simard</t>
+  </si>
+  <si>
+    <t>DescJeu de varchar(250) à varchar(350)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -203,6 +221,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -531,61 +550,61 @@
   <dimension ref="A2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:J2"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.21875" customWidth="1"/>
     <col min="2" max="3" width="14.88671875" customWidth="1"/>
-    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="4" max="4" width="36.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="14"/>
+      <c r="B2" s="15"/>
       <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="D2" s="6"/>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="14"/>
+      <c r="B3" s="15"/>
       <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="6"/>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="15"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="9" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="12"/>
     </row>
     <row r="5" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
+      <c r="B5" s="13"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13"/>
     </row>
     <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -605,18 +624,38 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="8">
+        <v>42257</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="8">
+        <v>42257</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>

</xml_diff>

<commit_message>
maj plein de trucs
</commit_message>
<xml_diff>
--- a/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
+++ b/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>ID du projet</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>DescJeu de varchar(250) à varchar(350)</t>
+  </si>
+  <si>
+    <t>GA02</t>
+  </si>
+  <si>
+    <t>NomJeu de varchar(30) à varchar(50)</t>
+  </si>
+  <si>
+    <t>EL01</t>
+  </si>
+  <si>
+    <t>Élodie Kérouak</t>
+  </si>
+  <si>
+    <t>Tag devient null</t>
   </si>
 </sst>
 </file>
@@ -550,7 +565,7 @@
   <dimension ref="A2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,18 +673,38 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8">
+        <v>42262</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="8">
+        <v>42262</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H11" s="5" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
maj de beaucoup de choses
</commit_message>
<xml_diff>
--- a/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
+++ b/Sprint 1/Global/S1_Suivi_Modifications_DBA.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>ID du projet</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Tag devient null</t>
+  </si>
+  <si>
+    <t>GA03</t>
+  </si>
+  <si>
+    <t>NomVersion de varchar(35) à varchar(50)</t>
   </si>
 </sst>
 </file>
@@ -565,7 +571,7 @@
   <dimension ref="A2:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,11 +716,21 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="8">
+        <v>42262</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="H12" t="s">
         <v>6</v>
       </c>

</xml_diff>